<commit_message>
Finished and ordered boards
</commit_message>
<xml_diff>
--- a/hardware/gerberfiles/ETG Ordering Files/SwitchBoardRev1BOM.xlsx
+++ b/hardware/gerberfiles/ETG Ordering Files/SwitchBoardRev1BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parker\Desktop\SeniorDesign\sddec21-07\hardware\gerberfiles\ETG Ordering Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A90C975-F3F2-4335-9D6D-FCEB3999AC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623C69A8-E10F-40C8-8AE1-85B85CCD9491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{362D0179-1D36-4F9A-8AB1-3CB748E57F0C}"/>
   </bookViews>
@@ -171,7 +171,7 @@
     <t>http://www.onsemi.com/pub_link/Collateral/NCP1117-D.PDF</t>
   </si>
   <si>
-    <t>488-NCP1117IST33T3GCT-ND</t>
+    <t>NCP1117ST33T3GOSCT-ND</t>
   </si>
 </sst>
 </file>
@@ -523,15 +523,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5CF021-6AE4-40C1-9373-CD0D85BA889B}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection sqref="A1:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -550,8 +550,12 @@
       <c r="F1">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1">
+        <f>F1*2+1</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -570,8 +574,12 @@
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <f t="shared" ref="G2:G13" si="0">F2*2+1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -590,8 +598,12 @@
       <c r="F3">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -610,8 +622,12 @@
       <c r="F4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -630,8 +646,12 @@
       <c r="F5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -650,8 +670,12 @@
       <c r="F6">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -667,8 +691,12 @@
       <c r="F7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -687,8 +715,12 @@
       <c r="F8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -707,8 +739,12 @@
       <c r="F9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -724,8 +760,12 @@
       <c r="F10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -741,8 +781,12 @@
       <c r="F11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -758,8 +802,12 @@
       <c r="F12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -777,6 +825,10 @@
       </c>
       <c r="F13">
         <v>1</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>